<commit_message>
🤖 Atualização automática local — 03/06/2025 07:54:34
</commit_message>
<xml_diff>
--- a/Python/Asimov/Python Básico/Lendo e escrevendo arquivos/Módulo 03/planilhas/clientes.xlsx
+++ b/Python/Asimov/Python Básico/Lendo e escrevendo arquivos/Módulo 03/planilhas/clientes.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28730"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FAS\GitHub\Cursos\Python\Asimov\Python Básico\Lendo e escrevendo arquivos\Módulo 03\planilhas\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9960F63E-9A98-4186-9383-227FB282D57B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12330"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RS" sheetId="1" r:id="rId1"/>
@@ -1732,14 +1738,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
-  <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;_-;_-@_-"/>
-  </numFmts>
-  <fonts count="20">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <fonts count="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -1747,346 +1747,16 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="33">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -2094,251 +1764,9 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2347,89 +1775,158 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Moeda" xfId="2" builtinId="4"/>
-    <cellStyle name="Porcentagem" xfId="3" builtinId="5"/>
-    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
-    <cellStyle name="Moeda [0]" xfId="5" builtinId="7"/>
-    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
-    <cellStyle name="Hyperlink seguido" xfId="7" builtinId="9"/>
-    <cellStyle name="Observação" xfId="8" builtinId="10"/>
-    <cellStyle name="Texto de Aviso" xfId="9" builtinId="11"/>
-    <cellStyle name="Título" xfId="10" builtinId="15"/>
-    <cellStyle name="Texto Explicativo" xfId="11" builtinId="53"/>
-    <cellStyle name="Título 1" xfId="12" builtinId="16"/>
-    <cellStyle name="Título 2" xfId="13" builtinId="17"/>
-    <cellStyle name="Título 3" xfId="14" builtinId="18"/>
-    <cellStyle name="Título 4" xfId="15" builtinId="19"/>
-    <cellStyle name="Entrada" xfId="16" builtinId="20"/>
-    <cellStyle name="Saída" xfId="17" builtinId="21"/>
-    <cellStyle name="Cálculo" xfId="18" builtinId="22"/>
-    <cellStyle name="Célula de Verificação" xfId="19" builtinId="23"/>
-    <cellStyle name="Célula Vinculada" xfId="20" builtinId="24"/>
-    <cellStyle name="Total" xfId="21" builtinId="25"/>
-    <cellStyle name="Bom" xfId="22" builtinId="26"/>
-    <cellStyle name="Ruim" xfId="23" builtinId="27"/>
-    <cellStyle name="Neutro" xfId="24" builtinId="28"/>
-    <cellStyle name="Ênfase 1" xfId="25" builtinId="29"/>
-    <cellStyle name="20% - Ênfase 1" xfId="26" builtinId="30"/>
-    <cellStyle name="40% - Ênfase 1" xfId="27" builtinId="31"/>
-    <cellStyle name="60% - Ênfase 1" xfId="28" builtinId="32"/>
-    <cellStyle name="Ênfase 2" xfId="29" builtinId="33"/>
-    <cellStyle name="20% - Ênfase 2" xfId="30" builtinId="34"/>
-    <cellStyle name="40% - Ênfase 2" xfId="31" builtinId="35"/>
-    <cellStyle name="60% - Ênfase 2" xfId="32" builtinId="36"/>
-    <cellStyle name="Ênfase 3" xfId="33" builtinId="37"/>
-    <cellStyle name="20% - Ênfase 3" xfId="34" builtinId="38"/>
-    <cellStyle name="40% - Ênfase 3" xfId="35" builtinId="39"/>
-    <cellStyle name="60% - Ênfase 3" xfId="36" builtinId="40"/>
-    <cellStyle name="Ênfase 4" xfId="37" builtinId="41"/>
-    <cellStyle name="20% - Ênfase 4" xfId="38" builtinId="42"/>
-    <cellStyle name="40% - Ênfase 4" xfId="39" builtinId="43"/>
-    <cellStyle name="60% - Ênfase 4" xfId="40" builtinId="44"/>
-    <cellStyle name="Ênfase 5" xfId="41" builtinId="45"/>
-    <cellStyle name="20% - Ênfase 5" xfId="42" builtinId="46"/>
-    <cellStyle name="40% - Ênfase 5" xfId="43" builtinId="47"/>
-    <cellStyle name="60% - Ênfase 5" xfId="44" builtinId="48"/>
-    <cellStyle name="Ênfase 6" xfId="45" builtinId="49"/>
-    <cellStyle name="20% - Ênfase 6" xfId="46" builtinId="50"/>
-    <cellStyle name="40% - Ênfase 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Ênfase 6" xfId="48" builtinId="52"/>
   </cellStyles>
   <dxfs count="17">
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.799981688894314"/>
-          <bgColor theme="4" tint="0.799981688894314"/>
+          <fgColor theme="4" tint="0.79995117038483843"/>
+          <bgColor theme="4" tint="0.79995117038483843"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="4" tint="0.39994506668294322"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79995117038483843"/>
+          <bgColor theme="4" tint="0.79995117038483843"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="4" tint="0.39994506668294322"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <border>
+        <bottom style="thin">
+          <color theme="4" tint="0.39994506668294322"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color theme="1"/>
+      </font>
+      <border>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79995117038483843"/>
+          <bgColor theme="4" tint="0.79995117038483843"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.799981688894314"/>
-          <bgColor theme="4" tint="0.799981688894314"/>
+          <fgColor theme="4" tint="0.79995117038483843"/>
+          <bgColor theme="4" tint="0.79995117038483843"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <font>
-        <b val="1"/>
+        <b/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79995117038483843"/>
+          <bgColor theme="4" tint="0.79995117038483843"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color theme="4" tint="0.39994506668294322"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39994506668294322"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79995117038483843"/>
+          <bgColor theme="4" tint="0.79995117038483843"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="4" tint="0.39994506668294322"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79995117038483843"/>
+          <bgColor theme="4" tint="0.79995117038483843"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79995117038483843"/>
+          <bgColor theme="4" tint="0.79995117038483843"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
         <color theme="1"/>
       </font>
     </dxf>
     <dxf>
       <font>
-        <b val="1"/>
+        <b/>
         <color theme="1"/>
       </font>
     </dxf>
     <dxf>
       <font>
-        <b val="1"/>
+        <b/>
         <color theme="1"/>
       </font>
       <border>
@@ -2440,7 +1937,7 @@
     </dxf>
     <dxf>
       <font>
-        <b val="1"/>
+        <b/>
         <color theme="0"/>
       </font>
       <fill>
@@ -2468,154 +1965,40 @@
           <color theme="4"/>
         </bottom>
         <horizontal style="thin">
-          <color theme="4" tint="0.399975585192419"/>
+          <color theme="4" tint="0.39994506668294322"/>
         </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.799981688894314"/>
-          <bgColor theme="4" tint="0.799981688894314"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="4" tint="0.399975585192419"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.799981688894314"/>
-          <bgColor theme="4" tint="0.799981688894314"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="4" tint="0.399975585192419"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <border>
-        <bottom style="thin">
-          <color theme="4" tint="0.399975585192419"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="1"/>
-        <color theme="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="1"/>
-        <color theme="1"/>
-      </font>
-      <border>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.799981688894314"/>
-          <bgColor theme="4" tint="0.799981688894314"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.799981688894314"/>
-          <bgColor theme="4" tint="0.799981688894314"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="1"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.799981688894314"/>
-          <bgColor theme="4" tint="0.799981688894314"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="4" tint="0.399975585192419"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.399975585192419"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="1"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.799981688894314"/>
-          <bgColor theme="4" tint="0.799981688894314"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="4" tint="0.399975585192419"/>
-        </bottom>
       </border>
     </dxf>
   </dxfs>
   <tableStyles count="2" defaultTableStyle="TableStylePreset3_Accent1" defaultPivotStyle="PivotStylePreset2_Accent1">
     <tableStyle name="TableStylePreset3_Accent1" pivot="0" count="7" xr9:uid="{59DB682C-5494-4EDE-A608-00C9E5F0F923}">
-      <tableStyleElement type="wholeTable" dxfId="6"/>
-      <tableStyleElement type="headerRow" dxfId="5"/>
-      <tableStyleElement type="totalRow" dxfId="4"/>
-      <tableStyleElement type="firstColumn" dxfId="3"/>
-      <tableStyleElement type="lastColumn" dxfId="2"/>
-      <tableStyleElement type="firstRowStripe" dxfId="1"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="0"/>
+      <tableStyleElement type="wholeTable" dxfId="16"/>
+      <tableStyleElement type="headerRow" dxfId="15"/>
+      <tableStyleElement type="totalRow" dxfId="14"/>
+      <tableStyleElement type="firstColumn" dxfId="13"/>
+      <tableStyleElement type="lastColumn" dxfId="12"/>
+      <tableStyleElement type="firstRowStripe" dxfId="11"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="10"/>
     </tableStyle>
     <tableStyle name="PivotStylePreset2_Accent1" table="0" count="10" xr9:uid="{267968C8-6FFD-4C36-ACC1-9EA1FD1885CA}">
-      <tableStyleElement type="headerRow" dxfId="16"/>
-      <tableStyleElement type="totalRow" dxfId="15"/>
-      <tableStyleElement type="firstRowStripe" dxfId="14"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="13"/>
-      <tableStyleElement type="firstSubtotalRow" dxfId="12"/>
-      <tableStyleElement type="secondSubtotalRow" dxfId="11"/>
-      <tableStyleElement type="firstRowSubheading" dxfId="10"/>
-      <tableStyleElement type="secondRowSubheading" dxfId="9"/>
-      <tableStyleElement type="pageFieldLabels" dxfId="8"/>
-      <tableStyleElement type="pageFieldValues" dxfId="7"/>
+      <tableStyleElement type="headerRow" dxfId="9"/>
+      <tableStyleElement type="totalRow" dxfId="8"/>
+      <tableStyleElement type="firstRowStripe" dxfId="7"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="6"/>
+      <tableStyleElement type="firstSubtotalRow" dxfId="5"/>
+      <tableStyleElement type="secondSubtotalRow" dxfId="4"/>
+      <tableStyleElement type="firstRowSubheading" dxfId="3"/>
+      <tableStyleElement type="secondRowSubheading" dxfId="2"/>
+      <tableStyleElement type="pageFieldLabels" dxfId="1"/>
+      <tableStyleElement type="pageFieldValues" dxfId="0"/>
     </tableStyle>
   </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -2873,22 +2256,22 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52:D63"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9.09765625" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="20.7142857142857" customWidth="1"/>
-    <col min="2" max="2" width="16.8571428571429" customWidth="1"/>
+    <col min="1" max="1" width="20.69921875" customWidth="1"/>
+    <col min="2" max="2" width="16.8984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -3607,20 +2990,21 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37:D63"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9.09765625" defaultRowHeight="13"/>
+  <cols>
+    <col min="1" max="1" width="16.09765625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
@@ -4128,20 +3512,18 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D43"/>
   <sheetViews>
     <sheetView topLeftCell="A20" workbookViewId="0">
       <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9.09765625" defaultRowHeight="13"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
@@ -4747,20 +4129,18 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9.09765625" defaultRowHeight="13"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
@@ -5646,6 +5026,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>